<commit_message>
feat: update uidaho_urls.json and enhance cost-benefit analysis documentation
Add numerous new URLs to uidaho_urls.json for faculty and staff profiles, ensuring comprehensive coverage for data extraction. Revise the cost-benefit analysis in model-cost-benefit-analysis.md to reflect updated pricing for Google Gemini 2.0 Flash, clarifying its competitive position against other models. Enhance the spike documentation to detail the extraction process using foundation models, including metrics for accuracy and cost, and outline next steps for further evaluation and improvements.
</commit_message>
<xml_diff>
--- a/output/extracted_profiles_errors.xlsx
+++ b/output/extracted_profiles_errors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,14 +473,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>profile-thread-7388a4a3-91b5-42a4-a1e2-7b295561673c</t>
+          <t>profile-thread-b85ee111-52ab-430d-828a-e64be5aab7e4</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/people/mark-mcguire</t>
+          <t>https://www.uidaho.edu/cals/people/erinn-cruz</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -490,19 +490,19 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/people/mark-mcguire', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/people/mark-mcguire\n'}</t>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/people/erinn-cruz', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/people/erinn-cruz\n'}</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>profile-thread-149f4e6a-3b71-42e1-8e2d-781b89405e91</t>
+          <t>profile-thread-b40654af-c53d-4902-ba27-14a538a2e99e</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/paul-lewin</t>
+          <t>https://www.uidaho.edu/cals/people/mark-mcguire</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -512,19 +512,19 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/paul-lewin', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/paul-lewin\n'}</t>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/people/mark-mcguire', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/people/mark-mcguire\n'}</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>profile-thread-b3a8e2da-4b0c-49bd-a719-044545da9d42</t>
+          <t>profile-thread-0b30d9d6-7f46-438b-bde0-e0a14c0933bb</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/andrzej-paszczynski</t>
+          <t>https://www.uidaho.edu/cals/people/tenley-burke</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -534,34 +534,1354 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/andrzej-paszczynski', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/andrzej-paszczynski\n'}</t>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/people/tenley-burke', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/people/tenley-burke\n'}</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>profile-thread-6d6897ba-da41-42a9-b5bf-0b00e4783c79</t>
+          <t>profile-thread-ab9df044-8c62-4c0e-9038-cc9c069b0ff9</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>https://www.uidaho.edu/cals/agricultural-education-leadership-and-communications/our-people/clara-leigh-evans</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/agricultural-education-leadership-and-communications/our-people/clara-leigh-evans', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/agricultural-education-leadership-and-communications/our-people/clara-leigh-evans\n'}</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>profile-thread-d95c4e21-5795-4759-871c-686fde350582</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/paul-lewin</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/paul-lewin', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/agricultural-economics-and-rural-sociology/our-people/paul-lewin\n'}</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>profile-thread-d1d2dd84-956e-4a12-8b91-10795eec77c6</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/andrzej-paszczynski</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/andrzej-paszczynski', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/andrzej-paszczynski\n'}</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>profile-thread-8384a0db-1c67-4f4f-a886-6e5953fed8c7</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/barbara-nielsen</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Failed to fetch URL</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/barbara-nielsen', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/barbara-nielsen\n'}</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>profile-thread-0049fa1d-9edd-4f45-ad28-aef5bef13f4f</t>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>profile-thread-03627bf9-a7b4-4123-9a5d-00a3ce71738f</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/haedun-kim</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/haedun-kim', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/haedun-kim\n'}</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>profile-thread-5069c5db-f91a-49ea-b842-d5cb9b905a70</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/matt-powell</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/matt-powell', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/matt-powell\n'}</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>profile-thread-bfccc0a7-f986-46e6-83d4-5571a617557b</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/pedram-rezamand</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/pedram-rezamand', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/pedram-rezamand\n'}</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>profile-thread-34accbc1-8078-4718-92f5-0e5be0b84441</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/robert-collier</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/robert-collier', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/robert-collier\n'}</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>profile-thread-d27e3c1b-a9e8-4234-9105-3b59f9b95c8a</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/ronald-hardy</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/ronald-hardy', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/ronald-hardy\n'}</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>profile-thread-17877b31-722c-45da-82f8-a077b99b1f26</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/vikas-kumar</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/vikas-kumar', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/animal-veterinary-and-food-sciences/our-people/vikas-kumar\n'}</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>profile-thread-878b6782-e3d2-4d4e-8210-5f6204512c28</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/entomology-plant-pathology-and-nematology/our-people/saad-hafez</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/entomology-plant-pathology-and-nematology/our-people/saad-hafez', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/entomology-plant-pathology-and-nematology/our-people/saad-hafez\n'}</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>profile-thread-c24312e3-4807-40f8-b828-303155e441d5</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/family-and-consumer-sciences/our-people/trevor-white</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/family-and-consumer-sciences/our-people/trevor-white', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/family-and-consumer-sciences/our-people/trevor-white\n'}</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>profile-thread-c0cd31d4-84a3-4d1e-95f7-55e387757ffe</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/plant-sciences/our-people/jonah-kaya</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/plant-sciences/our-people/jonah-kaya', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/plant-sciences/our-people/jonah-kaya\n'}</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>profile-thread-79135d10-9d90-4981-9110-40b62e530fc8</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/plant-sciences/our-people/pamela-hutchinson</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/plant-sciences/our-people/pamela-hutchinson', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/plant-sciences/our-people/pamela-hutchinson\n'}</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>profile-thread-72d6b157-5a38-4d2c-97d4-5c2c78442d04</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/plant-sciences/our-people/prayusha-bhattarai</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/plant-sciences/our-people/prayusha-bhattarai', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/plant-sciences/our-people/prayusha-bhattarai\n'}</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>profile-thread-0cf2f4c9-9d16-4035-a870-e6224663ee7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/plant-sciences/our-people/randy-lawrence</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/plant-sciences/our-people/randy-lawrence', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/plant-sciences/our-people/randy-lawrence\n'}</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>profile-thread-ba56608c-1c60-4155-ab08-4acf1a5d81b1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/soil-and-water-systems/our-people/heather-ireton</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/soil-and-water-systems/our-people/heather-ireton', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/soil-and-water-systems/our-people/heather-ireton\n'}</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>profile-thread-16aa3ac7-f649-4cec-9d8c-69b37dda4e64</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/soil-and-water-systems/our-people/isabell-von-rein</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/soil-and-water-systems/our-people/isabell-von-rein', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/soil-and-water-systems/our-people/isabell-von-rein\n'}</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>profile-thread-cecdbb9a-3589-492f-91af-3f40b5a8acab</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/soil-and-water-systems/our-people/jane-lucas</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/soil-and-water-systems/our-people/jane-lucas', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/soil-and-water-systems/our-people/jane-lucas\n'}</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>profile-thread-c24ccbbd-9362-4287-91a7-0643bbe08fc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cals/seed-potato-germplasm-program/our-people/jenny-durrin</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cals/seed-potato-germplasm-program/our-people/jenny-durrin', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cals/seed-potato-germplasm-program/our-people/jenny-durrin\n'}</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>profile-thread-754d2393-88f5-4483-9c9f-837d3ec458fc</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/a-b/andrew-bingham</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/andrew-bingham', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/andrew-bingham\n'}</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>profile-thread-931fb58f-f916-4820-b231-4beb2d460cfa</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/a-b/erin-argyle</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/erin-argyle', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/erin-argyle\n'}</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>profile-thread-9aa0b20f-256b-4aee-983b-80f2e9e7dfd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/a-b/julie-buck</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/julie-buck', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/julie-buck\n'}</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>profile-thread-63d93f50-1ba1-4033-ab36-c57df1edd86f</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/a-b/madison-anderson</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/madison-anderson', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/madison-anderson\n'}</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>profile-thread-385e6bc0-5b77-4d19-8e53-81249ce5455a</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/a-b/susan-bell</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/susan-bell', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/susan-bell\n'}</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>profile-thread-023ea9fa-84ba-4594-a679-9d813adb212f</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/a-b/whitney-beard</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/whitney-beard', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/whitney-beard\n'}</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>profile-thread-098040f0-35af-409c-bd11-ab3895e322e7</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/a-b/cody-beus</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/cody-beus', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/a-b/cody-beus\n'}</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>profile-thread-7976ad7a-7c28-414b-bd3c-32f9f41b7fb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/jody-harrington</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/jody-harrington', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/jody-harrington\n'}</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>profile-thread-c392feed-e37e-4296-9e4b-af29379d0c38</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/kathyrn-hickok</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/kathyrn-hickok', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/kathyrn-hickok\n'}</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>profile-thread-5ad37d99-7fe5-4aba-8687-aa8815fba152</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/polly-grasham</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/polly-grasham', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/polly-grasham\n'}</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>profile-thread-d511a6f1-63aa-4e4a-9561-53667282d004</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/stephanie-hamblin</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/stephanie-hamblin', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/stephanie-hamblin\n'}</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>profile-thread-54330b07-a327-431c-a972-fac4c1af301c</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/danielle-evans</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/danielle-evans', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/danielle-evans\n'}</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>profile-thread-c96223c2-7dab-4f59-ae41-2b9e7998cbd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/kathy-garofano</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/kathy-garofano', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/kathy-garofano\n'}</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>profile-thread-75764c1e-ee17-4a53-b180-ad5a8398afa0</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/nav-ghimire</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/nav-ghimire', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/nav-ghimire\n'}</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>profile-thread-3634ecfd-9739-419b-987e-14e696fe41b0</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/ronda-hirnyck</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/ronda-hirnyck', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/ronda-hirnyck\n'}</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>profile-thread-e0656f6c-4230-4318-97bd-c011d86c2dc6</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/f-h/angie-freel</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/angie-freel', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/f-h/angie-freel\n'}</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>profile-thread-45be05f5-1527-45b7-a1d7-5f3f88505077</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/i-k/teri-johnson</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/i-k/teri-johnson', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/i-k/teri-johnson\n'}</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>profile-thread-91521003-d3c4-43bb-bf50-3a499ab28de7</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/l-o/shaina-nomee</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/shaina-nomee', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/shaina-nomee\n'}</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>profile-thread-49dc50c3-7bd3-44fc-8454-6c997094eb33</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/l-o/jennifer-matthews</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/jennifer-matthews', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/jennifer-matthews\n'}</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>profile-thread-f10f9698-6011-4c28-bb54-d5582df7f261</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/l-o/alyssa-brotnov</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/alyssa-brotnov', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/alyssa-brotnov\n'}</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>profile-thread-c3b3e1e7-8678-4357-9d12-cc85c55a8e61</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/l-o/hope-newman</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/hope-newman', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/hope-newman\n'}</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>profile-thread-3337da46-4586-438e-b8fc-5f639e61beff</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/l-o/jennifer-makinson</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/jennifer-makinson', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/l-o/jennifer-makinson\n'}</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>profile-thread-7059a4c0-aaa5-4a28-a16a-99138259ff87</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/p-r/sarah-ramirez</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/p-r/sarah-ramirez', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/p-r/sarah-ramirez\n'}</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>profile-thread-30cdbc59-c992-49ee-bab0-e06b9649b440</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/s-t/donna-schwarting</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/donna-schwarting', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/donna-schwarting\n'}</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>profile-thread-d48dfc10-e271-4734-b80f-a328589f1dd3</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/s-t/karen-trappet</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/karen-trappet', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/karen-trappet\n'}</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>profile-thread-10018d22-f567-47ec-bf29-c83a1fa91c07</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/s-t/kimberly-tate</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/kimberly-tate', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/kimberly-tate\n'}</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>profile-thread-c594d4a7-8ddf-43fa-8e9f-17b445005c01</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/s-t/madison-arnzen</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/madison-arnzen', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/madison-arnzen\n'}</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>profile-thread-6422265f-46e2-4b1d-b6fd-f92862f87eb0</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/s-t/maureen-toomey</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/maureen-toomey', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/maureen-toomey\n'}</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>profile-thread-c8e825fb-0ce8-4184-bd40-217a08c9c57a</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/s-t/taylor-smith</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/taylor-smith', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/s-t/taylor-smith\n'}</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>profile-thread-823a75ea-207e-4681-bb0f-65ab9a057f82</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/extension/our-people/u-z/julia-villagomez</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/u-z/julia-villagomez', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/extension/our-people/u-z/julia-villagomez\n'}</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>profile-thread-a7627d65-f488-4efc-a51d-e9760d750500</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cbe/our-people/accounting-mis-faculty/lela-pumphrey</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cbe/our-people/accounting-mis-faculty/lela-pumphrey', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cbe/our-people/accounting-mis-faculty/lela-pumphrey\n'}</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>profile-thread-34a459f4-6cfb-47ad-bb16-e8afd51670d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/law/people/faculty/dawn-young</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/dawn-young', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/dawn-young\n'}</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>profile-thread-6082c44f-caaf-4eb0-964b-0fe2ff9a8ee0</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/law/people/faculty/debmcin</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/debmcin', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/debmcin\n'}</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>profile-thread-58b964dd-3dd9-4bb7-bcc9-778e79ef6612</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/law/people/faculty/johanna-kalb</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/johanna-kalb', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/johanna-kalb\n'}</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>profile-thread-654a5186-6d55-4afd-afe3-dfa1e129a043</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/law/people/faculty/megan-starich</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/megan-starich', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/megan-starich\n'}</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>profile-thread-6cb9c4a1-294b-4eba-b116-7c4e9d6635c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/law/people/faculty/merritt-dublin</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/merritt-dublin', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/merritt-dublin\n'}</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>profile-thread-581794d5-1a80-4624-9e23-a5580a7b60d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/law/people/faculty/millers</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/millers', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/law/people/faculty/millers\n'}</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>profile-thread-d48c3ec6-a285-45aa-9aa9-6b8101fe35f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/class/csj/people/leah-evans-janke</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/class/csj/people/leah-evans-janke', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/class/csj/people/leah-evans-janke\n'}</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>profile-thread-f83d37fb-cb48-484c-8457-335a520baa74</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/cnr/departments/fish-and-wildlife-sciences/our-people/seunghan-lee</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/cnr/departments/fish-and-wildlife-sciences/our-people/seunghan-lee', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/cnr/departments/fish-and-wildlife-sciences/our-people/seunghan-lee\n'}</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>profile-thread-5b69cee1-f52d-406a-b6be-91b2a88751ec</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/sci/biology/people/adjuncts</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>LLM output failed validation/parsing after successful call</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'ValueError', 'message': 'LLM output is not a JSON object or a list containing a single object.', 'llm_content': '```json\n[\n  {\n    "first_name": "Tyler",\n    "middle_name": null,\n    "last_name": "Bland",\n    "title": "Affiliate Faculty",\n    "office": "WWAMI Medical Education Building 153B",\n    "phone": "208-885-1236",\n    "email": "tbland@uidaho.edu",\n    "college_unit": null,\n    "department_division": "Department of Biological Sciences",\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Rajal",\n    "middle_name": "G",\n    "last_name": "Cohen",\n    "title": "Affiliate Faculty Assistant Professor\\u00a0of Psychology &amp; Communication Studies Graduate Faculty in Human Factors and Neuroscience",\n    "office": null,\n    "phone": "208-885-4102",\n    "email": "rcohen@uidaho.edu",\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [\n      {\n        "degree_type": "Ph.D.",\n        "institution": null,\n        "year": null\n      }\n    ],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Courtney",\n    "middle_name": null,\n    "last_name": "Conway",\n    "title": "Affiliate Faculty Director of the Idaho Cooperative Fish &amp; Wildlife Research Unit",\n    "office": null,\n    "phone": "208-885-6176",\n    "email": "cconway@uidaho.edu",\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [\n      {\n        "degree_type": "Ph.D.",\n        "institution": null,\n        "year": null\n      }\n    ],\n    "research_focus_areas": [\n      "Behavioral Ecology of Birds and Mammals",\n      "Conservation Biology",\n      "Animal Migration",\n      "Life History Evolution"\n    ]\n  },\n  {\n    "first_name": "Alexandra",\n    "middle_name": null,\n    "last_name": "Fraik",\n    "title": "Adjunct Faculty",\n    "office": null,\n    "phone": null,\n    "email": "alexandra.fraik@usda.gov",\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Esteban",\n    "middle_name": null,\n    "last_name": "Hernandez-Vargas",\n    "title": "Affiliate Faculty",\n    "office": null,\n    "phone": "208-885-2188",\n    "email": "estaban@uidaho.edu",\n    "college_unit": null,\n    "department_division": "Department of Mathematics and Statistical Science",\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Patrick",\n    "middle_name": "J",\n    "last_name": "Hrdlicka",\n    "title": "Affiliate Faculty",\n    "office": null,\n    "phone": "208-885-0108",\n    "email": "hrdlicka@uidaho.edu",\n    "college_unit": null,\n    "department_division": "Department of Chemistry",\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Brian",\n    "middle_name": null,\n    "last_name": "Kennedy",\n    "title": "Affiliate Faculty",\n    "office": null,\n    "phone": "208-885-5171",\n    "email": "kennedy@uidaho.edu",\n    "college_unit": "College of Natural Resources",\n    "department_division": "Dept. of Fish &amp; Wildlife Resources",\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Peter",\n    "middle_name": null,\n    "last_name": "Meserve",\n    "title": "Adjunct Faculty Distinguished Research Professor, Northern Illinois University, Emeritus",\n    "office": null,\n    "phone": null,\n    "email": null,\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Andrew",\n    "middle_name": null,\n    "last_name": "Pierce",\n    "title": "Adjunct Faculty",\n    "office": null,\n    "phone": "208-885-8857",\n    "email": "apierce@uidaho.edu",\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Christopher",\n    "middle_name": null,\n    "last_name": "Remien",\n    "title": "Affiliate Faculty",\n    "office": null,\n    "phone": null,\n    "email": "cremien@uidaho.edu",\n    "college_unit": null,\n    "department_division": "Department of Mathematics",\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Nathan",\n    "middle_name": "R",\n    "last_name": "Schiele",\n    "title": null,\n    "office": "Engineering/Physics 412",\n    "phone": "208-885-9063",\n    "email": "nrschiele@uidaho.edu",\n    "college_unit": null,\n    "department_division": "Department of Biological Engineering",\n    "degrees": [],\n    "research_focus_areas": [\n      "Tissue Engineering",\n      "Mechanobiology",\n      "Musculoskeletal Tissues",\n      "Tendon Mechanics",\n      "Stem Cell Differentiation"\n    ]\n  },\n  {\n    "first_name": "Irvin",\n    "middle_name": "R",\n    "last_name": "Schultz",\n    "title": "Adjunct Faculty Toxicologist",\n    "office": null,\n    "phone": null,\n    "email": "irvin.schultz@noaa.gov",\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [],\n    "research_focus_areas": [\n      "Ecotoxicology and Biotechnology",\n      "Marine and Coastal Resources",\n      "Marine and Environmental Chemistry",\n      "Water Resources Modeling"\n    ]\n  },\n  {\n    "first_name": "Sergey",\n    "middle_name": null,\n    "last_name": "Stolyar",\n    "title": "Adjunct Faculty",\n    "office": null,\n    "phone": "206-931-8762",\n    "email": "sstolyar1717@gmail.com",\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "Dave",\n    "middle_name": null,\n    "last_name": "Tank",\n    "title": "Adjunct Faculty",\n    "office": null,\n    "phone": "307-766-2384",\n    "email": "dtank@uwyo.edu",\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [],\n    "research_focus_areas": []\n  },\n  {\n    "first_name": "JT",\n    "middle_name": null,\n    "last_name": "Van Leuven",\n    "title": "Affiliate Faculty",\n    "office": null,\n    "phone": null,\n    "email": "jvanleuven@uidaho.edu",\n    "college_unit": null,\n    "department_division": null,\n    "degrees": [],\n    "research_focus_areas": []\n  }\n]\n```', 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 452, in extract_data\n    raise ValueError(\nValueError: LLM output is not a JSON object or a list containing a single object.\n'}</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>profile-thread-57969053-7325-418b-8f46-0e2b0db21d48</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>https://www.uidaho.edu/sci/physics/people/faculty/machleid</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Failed to fetch URL</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>{'exception_type': 'HTTPError', 'message': '404 Client Error: Not Found for url: https://www.uidaho.edu/sci/physics/people/faculty/machleid', 'status_code': 404, 'traceback': 'Traceback (most recent call last):\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/src/nodes.py", line 88, in fetch_html\n    response.raise_for_status()  # Raise HTTPError for bad responses (4xx or 5xx)\n  File "/Users/colesummers/Documents/GitHub/profile-extractor/.venv/lib/python3.9/site-packages/requests/models.py", line 1024, in raise_for_status\n    raise HTTPError(http_error_msg, response=self)\nrequests.exceptions.HTTPError: 404 Client Error: Not Found for url: https://www.uidaho.edu/sci/physics/people/faculty/machleid\n'}</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>profile-thread-c34c3db7-ad32-47cf-85a9-64f1a848f19a</t>
         </is>
       </c>
     </row>

</xml_diff>